<commit_message>
Global spatial autocorrelation for census tracts and grid polygons
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/doc/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/doc/Townes_SOC5670_Homework01_Tables.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOC5670\Assignments\Homework01\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOC5670\Assignments\Homework01\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830"/>
   </bookViews>
   <sheets>
     <sheet name="DirectionalDistribution" sheetId="1" r:id="rId1"/>
     <sheet name="SpatialAutocorrelation" sheetId="2" r:id="rId2"/>
+    <sheet name="GlobalSpatialAutocorrComparison" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>Variable</t>
   </si>
@@ -89,18 +90,6 @@
     <t>Directional Distribution</t>
   </si>
   <si>
-    <t>Table #. Spatial Descriptive Statistics for the St. Louis Metropolitan Statistical Area</t>
-  </si>
-  <si>
-    <t>Variable 1</t>
-  </si>
-  <si>
-    <t>Variable 2</t>
-  </si>
-  <si>
-    <t>Variable 3</t>
-  </si>
-  <si>
     <t>Significance</t>
   </si>
   <si>
@@ -110,24 +99,12 @@
     <t>***</t>
   </si>
   <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>*** p &lt; 0.001, ** p &lt; 0.01, * p &lt; 0.05</t>
   </si>
   <si>
-    <t>Queen method used for weight matrix.</t>
-  </si>
-  <si>
     <t>Source: U.S. Census ACS 2014-2018 5-year estimate. Table created by Author.</t>
   </si>
   <si>
-    <t>Table #. Spatial Autocorrelation of Regression Model Variables</t>
-  </si>
-  <si>
     <t>z-value</t>
   </si>
   <si>
@@ -137,21 +114,107 @@
     <t>Source: U.S. Census ACS 2014-2018 5-year estimates. Table created by Author.</t>
   </si>
   <si>
-    <t>Variable 4</t>
-  </si>
-  <si>
-    <t>Variable 5</t>
-  </si>
-  <si>
-    <t>Variable 6</t>
+    <t>Grid Polygons (1,000 meter X 1,000 meter)</t>
+  </si>
+  <si>
+    <t>pblk_grid</t>
+  </si>
+  <si>
+    <t>pwht_grid</t>
+  </si>
+  <si>
+    <t>pwht</t>
+  </si>
+  <si>
+    <t>pblk</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Table #. Comparison of Global Spatial Autocorrelation of Select Regression Model Variables</t>
+  </si>
+  <si>
+    <t>Census Tract Polygons</t>
+  </si>
+  <si>
+    <t>Queen method used for contiguity weight matrix.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>edtot</t>
+  </si>
+  <si>
+    <t>pov</t>
+  </si>
+  <si>
+    <t>mhi</t>
+  </si>
+  <si>
+    <t>nhi</t>
+  </si>
+  <si>
+    <t>Poverty</t>
+  </si>
+  <si>
+    <t>White population</t>
+  </si>
+  <si>
+    <t>Black population</t>
+  </si>
+  <si>
+    <t>Mean household income</t>
+  </si>
+  <si>
+    <t>No health insurance</t>
+  </si>
+  <si>
+    <t>Table #. Global Spatial Autocorrelation of Regression Model Variables Using Census Tracts Polygons</t>
+  </si>
+  <si>
+    <t>theil</t>
+  </si>
+  <si>
+    <t>index01</t>
+  </si>
+  <si>
+    <t>index02</t>
+  </si>
+  <si>
+    <t>Theil index of income inequality</t>
+  </si>
+  <si>
+    <t>Education attainment index</t>
+  </si>
+  <si>
+    <t>Index with ed., inequality, &amp; income equally weighted</t>
+  </si>
+  <si>
+    <t>Index with ed., inequality, &amp; income weighted 50%, 25%, &amp; 25%</t>
+  </si>
+  <si>
+    <t>Percent Black</t>
+  </si>
+  <si>
+    <t>Percent White</t>
+  </si>
+  <si>
+    <t>Table #. Spatial Descriptive Statistics for the Springfield, Missouri Metropolitan Statistical Area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -178,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -204,11 +267,147 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -257,6 +456,76 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -587,7 +856,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -678,7 +947,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -699,141 +968,508 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="26">
+        <v>0.54</v>
+      </c>
+      <c r="D3" s="24">
+        <v>9.4376999999999995</v>
+      </c>
+      <c r="E3" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="26">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D4" s="24">
+        <v>5.0582000000000003</v>
+      </c>
+      <c r="E4" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="26">
+        <v>0.46</v>
+      </c>
+      <c r="D5" s="24">
+        <v>7.9462000000000002</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="26">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="D6" s="24">
+        <v>8.3498999999999999</v>
+      </c>
+      <c r="E6" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="26">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="D7" s="24">
+        <v>8.0066000000000006</v>
+      </c>
+      <c r="E7" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="B8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="D8" s="24">
+        <v>8.2940000000000005</v>
+      </c>
+      <c r="E8" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="D9" s="24">
+        <v>9.2829999999999995</v>
+      </c>
+      <c r="E9" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="D10" s="24">
+        <v>8.5184999999999995</v>
+      </c>
+      <c r="E10" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="27">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="D11" s="25">
+        <v>5.3368000000000002</v>
+      </c>
+      <c r="E11" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1"/>
+    <col min="8" max="12" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="28"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="H3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="26">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="D4" s="24">
+        <v>8.2940000000000005</v>
+      </c>
+      <c r="E4" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="26">
+        <v>0.874</v>
+      </c>
+      <c r="J4" s="24">
+        <v>154.70519999999999</v>
+      </c>
+      <c r="K4" s="22">
+        <v>1E-3</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="27">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="D5" s="25">
+        <v>8.0066000000000006</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="J5" s="25">
+        <v>158.20840000000001</v>
+      </c>
+      <c r="K5" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Began paper for Homework01
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/doc/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/doc/Townes_SOC5670_Homework01_Tables.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795"/>
   </bookViews>
   <sheets>
     <sheet name="DirectionalDistribution" sheetId="1" r:id="rId1"/>
     <sheet name="GlobalSpatialAutocorrelation" sheetId="2" r:id="rId2"/>
     <sheet name="GlobalSpatialAutocorrComparison" sheetId="3" r:id="rId3"/>
+    <sheet name="GlobalSpatialAutocorrBivariate" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>Variable</t>
   </si>
@@ -93,9 +94,6 @@
     <t>***</t>
   </si>
   <si>
-    <t>*** p &lt; 0.001, ** p &lt; 0.01, * p &lt; 0.05</t>
-  </si>
-  <si>
     <t>Source: U.S. Census ACS 2014-2018 5-year estimate. Table created by Author.</t>
   </si>
   <si>
@@ -207,10 +205,58 @@
     <t>Components</t>
   </si>
   <si>
-    <t>Comparison of Global Spatial Autocorrelation of Select Regression Model Variables</t>
-  </si>
-  <si>
     <t>Global Spatial Autocorrelation of Regression Model Variables Using Census Tracts Polygons</t>
+  </si>
+  <si>
+    <t>Variable 1 Name</t>
+  </si>
+  <si>
+    <t>Variable 1 Description</t>
+  </si>
+  <si>
+    <t>Varable 2 Name</t>
+  </si>
+  <si>
+    <t>Variable 2 Description</t>
+  </si>
+  <si>
+    <t>Percent white population</t>
+  </si>
+  <si>
+    <t>Percent black population</t>
+  </si>
+  <si>
+    <t>Comparison of Univariate Global Spatial Autocorrelation of Select Regression Model Variables</t>
+  </si>
+  <si>
+    <t>Bivariate Global Spatial Autocorrelation of Regression Model Variables Using Census Tracts Polygons</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*** p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.001, ** p ≤ 0.01, * p ≤ 0.05</t>
+    </r>
+  </si>
+  <si>
+    <t>*** p ≤ 0.001, ** p ≤ 0.01, * p ≤ 0.05</t>
   </si>
 </sst>
 </file>
@@ -222,9 +268,9 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +292,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -423,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -510,13 +562,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -534,26 +607,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -884,34 +939,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-    </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
@@ -924,40 +979,40 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="30">
         <v>476624.581427</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="30">
         <v>476939.12674899999</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="30">
         <v>473977.381995</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="30">
         <v>475135.63196299999</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="30">
         <v>4119126.7492479999</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="30">
         <v>4118697.1233649999</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="30">
         <v>4116847.817572</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="30">
         <v>4116702.2038190002</v>
       </c>
     </row>
@@ -970,92 +1025,92 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="38">
+        <v>46</v>
+      </c>
+      <c r="C7" s="30">
         <v>9.6719570000000008</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="30">
         <v>2.632361</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="30">
         <v>152.314719</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="30">
         <v>177.25980000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="31">
         <v>17622.103956999999</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="31">
         <v>19964.432875999999</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="31">
         <v>11862.588578999999</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F8" s="31">
         <v>15781.394719</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="31">
         <v>21397.015105999999</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="31">
         <v>27396.548221000001</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="31">
         <v>13886.793740999999</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="31">
         <v>23257.142437999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="32">
         <f>1184506679.1946/1000000</f>
         <v>1184.5066791946001</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="32">
         <f>1718213889.26599/1000000</f>
         <v>1718.21388926599</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="32">
         <f>517497730.280002/1000000</f>
         <v>517.49773028000197</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="32">
         <f>1152986789.7537/1000000</f>
         <v>1152.9867897537001</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="A11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1074,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1085,47 +1140,47 @@
     <col min="3" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>48</v>
+    <row r="1" spans="1:6" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="A2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="45" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="18">
         <v>0.54</v>
@@ -1142,10 +1197,10 @@
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="18">
         <v>0.28499999999999998</v>
@@ -1162,10 +1217,10 @@
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="18">
         <v>0.46</v>
@@ -1182,10 +1237,10 @@
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="18">
         <v>0.48599999999999999</v>
@@ -1202,10 +1257,10 @@
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="18">
         <v>0.48599999999999999</v>
@@ -1222,10 +1277,10 @@
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="18">
         <v>0.46500000000000002</v>
@@ -1242,10 +1297,10 @@
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="18">
         <v>0.56899999999999995</v>
@@ -1262,10 +1317,10 @@
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="18">
         <v>0.50800000000000001</v>
@@ -1282,10 +1337,10 @@
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="19">
         <v>0.29199999999999998</v>
@@ -1301,34 +1356,34 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
+      <c r="A13" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
+      <c r="A14" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
+      <c r="A15" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1356,47 +1411,47 @@
     <col min="8" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>48</v>
+    <row r="1" spans="1:12" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="A2" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
+      <c r="B3" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="29"/>
-      <c r="H3" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="37"/>
+      <c r="H3" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="44"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>0</v>
@@ -1405,10 +1460,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>11</v>
@@ -1421,10 +1476,10 @@
         <v>12</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="L4" s="27" t="s">
         <v>11</v>
@@ -1432,10 +1487,10 @@
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="18">
         <v>0.46500000000000002</v>
@@ -1451,7 +1506,7 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" s="18">
         <v>0.874</v>
@@ -1468,10 +1523,10 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="19">
         <v>0.48599999999999999</v>
@@ -1487,7 +1542,7 @@
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="19">
         <v>0.9</v>
@@ -1503,52 +1558,52 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="A7" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
+      <c r="A8" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
+      <c r="A9" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>
@@ -1586,4 +1641,216 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="8" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="18">
+        <v>-0.248</v>
+      </c>
+      <c r="F4" s="16">
+        <v>-5.5247000000000002</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="18">
+        <v>-0.21299999999999999</v>
+      </c>
+      <c r="F5" s="16">
+        <v>-4.7365000000000004</v>
+      </c>
+      <c r="G5" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="18">
+        <v>-0.499</v>
+      </c>
+      <c r="F6" s="16">
+        <v>-9.1736000000000004</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="19">
+        <v>0.248</v>
+      </c>
+      <c r="F7" s="17">
+        <v>5.7842000000000002</v>
+      </c>
+      <c r="G7" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tables and Figures 1 through 5 to Homework01 paper
</commit_message>
<xml_diff>
--- a/Assignments/Homework01/doc/Townes_SOC5670_Homework01_Tables.xlsx
+++ b/Assignments/Homework01/doc/Townes_SOC5670_Homework01_Tables.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="4830" tabRatio="795"/>
   </bookViews>
   <sheets>
-    <sheet name="DirectionalDistribution" sheetId="1" r:id="rId1"/>
-    <sheet name="GlobalSpatialAutocorrelation" sheetId="2" r:id="rId2"/>
-    <sheet name="GlobalSpatialAutocorrComparison" sheetId="3" r:id="rId3"/>
+    <sheet name="SourceData" sheetId="5" r:id="rId1"/>
+    <sheet name="DirectionalDistribution" sheetId="1" r:id="rId2"/>
+    <sheet name="GlobalSpatialAutocorrelation" sheetId="2" r:id="rId3"/>
     <sheet name="GlobalSpatialAutocorrBivariate" sheetId="4" r:id="rId4"/>
+    <sheet name="GlobalSpatialAutocorrComparison" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
   <si>
     <t>Variable</t>
   </si>
@@ -127,9 +128,6 @@
     <t>Census Tract Polygons</t>
   </si>
   <si>
-    <t>Queen method used for contiguity weight matrix.</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -193,9 +191,6 @@
     <t>Angle of Rotation (degrees)</t>
   </si>
   <si>
-    <t>Table #</t>
-  </si>
-  <si>
     <t>Spatial Descriptive Statistics for the Springfield, Missouri Metropolitan Statistical Area</t>
   </si>
   <si>
@@ -221,9 +216,6 @@
   </si>
   <si>
     <t>Percent white population</t>
-  </si>
-  <si>
-    <t>Percent black population</t>
   </si>
   <si>
     <t>Comparison of Univariate Global Spatial Autocorrelation of Select Regression Model Variables</t>
@@ -258,6 +250,96 @@
   <si>
     <t>*** p ≤ 0.001, ** p ≤ 0.01, * p ≤ 0.05</t>
   </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>A02001</t>
+  </si>
+  <si>
+    <t>Sex, Total Population</t>
+  </si>
+  <si>
+    <t>A01001</t>
+  </si>
+  <si>
+    <t>Age, Total Population</t>
+  </si>
+  <si>
+    <t>A04001</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino by Race</t>
+  </si>
+  <si>
+    <t>A12001</t>
+  </si>
+  <si>
+    <t>Educational Attainment for Population 25 Years and Over</t>
+  </si>
+  <si>
+    <t>A14001</t>
+  </si>
+  <si>
+    <t>Household Income</t>
+  </si>
+  <si>
+    <t>A14006</t>
+  </si>
+  <si>
+    <t>Median Household Income</t>
+  </si>
+  <si>
+    <t>A13004</t>
+  </si>
+  <si>
+    <t>Ratio of Income in to Poverty Level</t>
+  </si>
+  <si>
+    <t>A20001</t>
+  </si>
+  <si>
+    <t>Health Insurance</t>
+  </si>
+  <si>
+    <t>Source: U.S. Census ACS 2014-2018 5-year estimate retrieved from SocialExplorer.com. Table created by Author.</t>
+  </si>
+  <si>
+    <t>Level of Measurement</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>Source Demographic Data</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Percent Black population</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>Table 5</t>
+  </si>
+  <si>
+    <t>Queen method (first order) used for contiguity weight matrix.</t>
+  </si>
 </sst>
 </file>
 
@@ -270,7 +352,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +381,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -308,7 +398,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -470,12 +560,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -574,6 +679,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -607,8 +721,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -925,61 +1080,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="48"/>
+    </row>
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+    </row>
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="6" width="20.7109375" customWidth="1"/>
+    <col min="3" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-    </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="B3" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="55" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -999,7 +1296,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1025,11 +1322,11 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="38" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="30">
         <v>9.6719570000000008</v>
@@ -1045,7 +1342,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1360,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1081,7 +1378,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -1103,14 +1400,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1125,13 +1422,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1142,45 +1437,45 @@
   <sheetData>
     <row r="1" spans="1:6" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="A2" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="35" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="18">
         <v>0.54</v>
@@ -1197,10 +1492,10 @@
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="18">
         <v>0.28499999999999998</v>
@@ -1217,10 +1512,10 @@
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="18">
         <v>0.46</v>
@@ -1237,10 +1532,10 @@
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="18">
         <v>0.48599999999999999</v>
@@ -1260,7 +1555,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="18">
         <v>0.48599999999999999</v>
@@ -1280,7 +1575,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="18">
         <v>0.46500000000000002</v>
@@ -1297,10 +1592,10 @@
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="18">
         <v>0.56899999999999995</v>
@@ -1317,10 +1612,10 @@
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="18">
         <v>0.50800000000000001</v>
@@ -1337,10 +1632,10 @@
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="19">
         <v>0.29199999999999998</v>
@@ -1356,34 +1651,34 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
+      <c r="A14" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+      <c r="A15" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1396,186 +1691,173 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" customWidth="1"/>
-    <col min="8" max="12" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-    </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="44"/>
-    </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="H3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="18">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="D5" s="16">
-        <v>8.2940000000000005</v>
-      </c>
-      <c r="E5" s="14">
+      <c r="D4" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="18">
+        <v>-0.248</v>
+      </c>
+      <c r="F4" s="16">
+        <v>-5.5247000000000002</v>
+      </c>
+      <c r="G4" s="14">
         <v>1E-3</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="H4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="18">
-        <v>0.874</v>
-      </c>
-      <c r="J5" s="16">
-        <v>154.70519999999999</v>
-      </c>
-      <c r="K5" s="14">
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="18">
+        <v>-0.21299999999999999</v>
+      </c>
+      <c r="F5" s="16">
+        <v>-4.7365000000000004</v>
+      </c>
+      <c r="G5" s="14">
         <v>1E-3</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="19">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="D6" s="17">
-        <v>8.0066000000000006</v>
-      </c>
-      <c r="E6" s="15">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="18">
+        <v>-0.499</v>
+      </c>
+      <c r="F6" s="16">
+        <v>-9.1736000000000004</v>
+      </c>
+      <c r="G6" s="14">
         <v>1E-3</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="H6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="19">
-        <v>0.9</v>
-      </c>
-      <c r="J6" s="17">
-        <v>158.20840000000001</v>
-      </c>
-      <c r="K6" s="15">
+    </row>
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="19">
+        <v>0.248</v>
+      </c>
+      <c r="F7" s="17">
+        <v>5.7842000000000002</v>
+      </c>
+      <c r="G7" s="15">
         <v>1E-3</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="H7" s="24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>61</v>
       </c>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
@@ -1584,26 +1866,257 @@
       <c r="F8" s="41"/>
       <c r="G8" s="41"/>
       <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59"/>
+      <c r="B3" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="47"/>
+    </row>
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="56"/>
+      <c r="H4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="D5" s="16">
+        <v>8.2940000000000005</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="57"/>
+      <c r="H5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="18">
+        <v>0.874</v>
+      </c>
+      <c r="J5" s="16">
+        <v>154.70519999999999</v>
+      </c>
+      <c r="K5" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="D6" s="17">
+        <v>8.0066000000000006</v>
+      </c>
+      <c r="E6" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="58"/>
+      <c r="H6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="J6" s="17">
+        <v>158.20840000000001</v>
+      </c>
+      <c r="K6" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
+      <c r="A9" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>
@@ -1641,216 +2154,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="8" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="33" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="18">
-        <v>-0.248</v>
-      </c>
-      <c r="F4" s="16">
-        <v>-5.5247000000000002</v>
-      </c>
-      <c r="G4" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="18">
-        <v>-0.21299999999999999</v>
-      </c>
-      <c r="F5" s="16">
-        <v>-4.7365000000000004</v>
-      </c>
-      <c r="G5" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="18">
-        <v>-0.499</v>
-      </c>
-      <c r="F6" s="16">
-        <v>-9.1736000000000004</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="19">
-        <v>0.248</v>
-      </c>
-      <c r="F7" s="17">
-        <v>5.7842000000000002</v>
-      </c>
-      <c r="G7" s="15">
-        <v>1E-3</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>